<commit_message>
Testing On Multiple Videos
</commit_message>
<xml_diff>
--- a/youtube_videos.xlsx
+++ b/youtube_videos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,67 +489,48 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://youtu.be/dQw4w9WgXcQ</t>
+          <t>https://youtu.be/VioF7v8Mikg?si=63mivZji4BTP0Goj</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[♪♪♪] ♪ We're no strangers to love ♪ ♪ You know the rules
-and so do I ♪ ♪ A full commitment's
-what I'm thinking of ♪ ♪ You wouldn't get this
-from any other guy ♪ ♪ I just wanna tell you
-how I'm feeling ♪ ♪ Gotta make you understand ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ We've known each other
-for so long ♪ ♪ Your heart's been aching
-but you're too shy to say it ♪ ♪ Inside we both know
-what's been going ♪ ♪ We know the game
-and we're gonna play it ♪ ♪ And if you ask me
-how I'm feeling ♪ ♪ Don't tell me
-you're too blind to see ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ Never gonna give you up ♪</t>
+          <t>Have you ever tried asking who won the IPL in 2025 [Music] or explain the code I wrote last week and what happens? Nine times out of 10 it just starts hallucinated just making stuff up going completely off the rails. Well, if you used any LLM in the past years, whether it's chat GPT, Claude, Gemini, Grock, Mistral, whatever, you've probably run into this one big annoying problem. You ask something super specific like a detailed question, something about yourself, some code you wrote last week or a spreadsheet that you uploaded and the model answers super confidently, like it knows everything, but it completely misses the point. Sometimes it just straight up hallucinates and gives answers that don't even exist. And look, the reason is dead simple. Large language models are pattern matching machines. They're incredible at regurgitating what they've already been trained on. But here's the kicker. They don't know your data, your context, or your secret source. And this is exactly why AI is still struggling to make a massive dent in fields like law, medicine, and compliance. You know, the places where hallucination isn't just an oops, my bad kind of situation. It's downright dangerous. Because let's be real, when you yank out your context, that fancy AI model just becomes generic. It becomes mid. But there's got to be a fix for this, right? We can't be pushing AI this hard and just leave this massive huge problem hanging. So, what are we going to do? We've actually got two solid ways to tackle this. And today, we're going to break them down for you. Ways of fixing AI. All right, so we've got this context problem. How do we actually solve it? It turns out that we've got two main players in the book. So, let's dissect them. The first option that we have is fine-tuning. Think of this as sending your AI model back to school. But this time, the curriculum is all about you. You literally take that base model and retrain it from the ground up with your own data. Like your emails, your entire code base, your chats, your pictures, everything gets thrown into the mix and it literally learns your specific domain and becomes a native. The upside is massive. Once the model is trained up, it's like it was literally born for your use cases. You don't need to keep spoon feeding it and giving it extra context every single time. It just gets it. but and it's a big butt. It can be extremely painful. Seriously. So, GPU time is going to cost you an arm and a leg. And what happens when your data changes? New data, new code, you guessed it, back to square one. Repeat the entire process. And plus, managing versions of these huge model checkpoints is a messy logistical nightmare. Trust me. So, that brings us to option number two, which is RAG. And RAG stands for retrieval augmented generation. And folks, this is where things get really, really interesting. This is the street smart agile cousin. Way way simpler. You don't even need to touch the underlying base model. No expensive retraining. Instead, you just build the clever context engine. And you can just think of this as a superefficient research assistant that sits around the LLM. And then at runtime, when a query comes in, the engine zips in and feeds the model just the right pieces of information it needs right when it needs them. Let's imagine that you're a world-class chef. You know how to cook anything, but you don't know what the next order from the dining room is going to be. With Rag, the moment that order hits the kitchen, bam, someone magically hands you the perfect detailed recipe for the exact dish. You didn't even have to deal on cooking. You just got the precise instructions that you needed. That is Rag right there. That's the power. No retraining, live updates, and way cheaper. So, now you guys understand the beauty of Rag. But why does this setup work so incredibly well? Why is it becoming the go-to for so many people trying to make LLMs actually useful with their own data? Why does Rag work so well? And here are the reasons. Number one is fast iterations, new docs, no sweat. Add them. Re-mbed them and your rag will instantly get smarter. No waiting for weeks for a retrain. Next is cheap infrastructure. Forget burning cash on endless GPU cycles. Rag is lean, minimal compute and your wallet will always stay happy. Next is it's always fresh. Your info never gets stale. upload a doc, your rag adapts in seconds and always with the latest intel. So you get speed, you can save cash, and your AI always stays current. That's a pretty powerful combo. Okay, so now you're probably thinking, okay, this sounds cool, but how does this rag magic actually work under the hood? Don't worry, we've got you. Rag pipeline. Okay, so how does this rag wizardry pull off giving your LM the brains it needs without the pain of retraining? We're going to break down the entire pipeline. And to make sure it's super easy to lock into your memory, we're going to use an analogy. Imagine you're setting up the most insanely organized high- techch library ever built. And for all you visual thinkers out there, we've created this crazy crazy massive diagram. So, we're going to drop a link so you can explore it on your own later, but for now, let's walk through it together. All right, let's dive in. All right, so step number one is your data intake. Imagine this being the part where the books arrive at the library. The first things first, your data. This is where all your books start showing up at the library doors. Think of your company's PDFs, your email archives, critical CSVs, even your entire codebase, all your content. So consider this to be your raw materials, the books that need to be cataloged in our super library. Now we move on to step two, which is chunking. Now imagine this is where you're breaking down the books into index cards. Now you're not just going to cram the entire encyclopedia onto one shelf, right? So, you take each book, each document, and you chunk it. You break it down into smaller bite-sized pieces. And you can think of them as individual index cards, maybe one paragraph per card or logical section. And the key is digestible pieces. Why? So, instead of your AI librarian having to flip through 300 pages to find a single answer, it can search these cards way faster and way more effectively. Precision, people, it's all about precision. So the tools that you can use for this is lang text split or you can also use llama index. Now we're moving on to step three which is embedding. Now imagine this to be the part where you're giving each card GPS coordinates. Now this is where the real AI magic starts to kick in. We take those text chunks, those index cards and we run them into coordinates. Now think of it as assigning a super precise GPS location to every single piece of information in your library but for language. The trick is that the cards with similar meaning get plotted in nearby locations in this massive multi-dimensional space. So words like similar, same, identical, they're all hanging out in the same neighborhood. Popular models that you can use for this is Google's text embedding API or you can also use OpenAI's text embedding 3. So you have a lot of horsepower to choose from. Now we're moving on to step number four, which is vector storage. Now this you can imagine as organizing the high-tech shelves. All right, so our Index cars now have their GPS coordinates. So, next up, we're going to need some serious shelving to store them. And this isn't your grandma's dusty bookshelf. This is a high performance vector database. So, you've got names like Pine Corn, Chroma, Qentrint in the Ring. Pick the one whose landing page you vibe with the most or the one that fits your scale and budget. Seriously, they're all pretty good. And it doesn't matter if you got a,000 cards or 10 million. These databases are built for speed. They can use semantic searches, finding those relevant meaning coordinates in milliseconds. Blink and you'll probably miss it. Okay, now we're moving on to step number five which is retrieval. Imagine this to be the part where the librarian finds the exact cards. Okay, so now your library is set up. Now user walks in with a question. So after the user asks that questions, what do you think is going to happen? So first the rag system takes that user's query, embeds it and turns it into a vector just like it did with all your documents. Then it performs a similarity search against your entire vector database and does something like show me the top five or six cards whose content is semantically closest to this question. So those are going to be your golden index cards with each one of them holding a crucial part of the answer and also a relevant snippet of information. Now we're moving on to step number six which is synthesis. This is the part where the librarian writes the perfect answer. This is where our super smart LLM, our AI librarian steps up to the plate. We feed it those top rank relevant chunks plus the original user query and we usually give it a little nudge, a guardrail prompt so to speak, something like use only the context provided. If the answer isn't there, just say so. The LLM then reads these carefully selected cards, understands the question in that specific context, and spits out focused, accurate, and contextual answer. No hallucination, no wild guessing, and no making stuff up. It's answering like it knows your data because in that moment, for that query, thanks to Rag, it actually does. So now, theory is great. Analogies are fun, but at Builder Central, we're all about building and shipping. So, now that we've walked you through how Ragg actually works, how about we show you what we actually built using the same exact approach. Ragbot, this isn't a full-blown line by line coding tutorial on how we built this specific chatbot. So, we actually dove deep into any which was our main tool for this in a previous video. If you've missed that video, make sure you check it out. The link is going to be either in the description or somewhere over here, depends on where the editor puts it. So, we showed how you can visually build these kind of powerful workflows with minimal to no code. So here's our flow for the data source. What we did is we used Google Drive and connected it via GCP. Now the reason we did this is because it enables us to upload the documents in real time effectively turning it into a live database. For embeddings we used OpenAI to generate them which was really really easy and inexpensive. For storage we use Pine Cone as our main vector storage database because they offer a fairly generous free storage tier. For retrieval and synthesis, we use Google's API, which handled the LLM part by synthesizing answers based on the embedded chunks that were received. So, what does this actually look like in action? Well, with this setup, you can throw pretty much any file at it. PDFs, Word docs, you name it. The bot chews it up, processes it, and then boom, you're chatting with your own data. So, you need to ask it something specific like, "What's the difference between function A and function B in this massive codebase I just uploaded?" And it should spit back the answer according to the document. It also works for CVs if you're hiring. So those complicated recipes you can never follow, dense legal documents, your chaotic lecture notes, whatever you've got, just, you know, be smart about it. Don't upload some deepest darkest secrets. Okay, that's kind of stupid. Don't do that. So what would be the end result? You can literally just drag and drop any document into the Google Drive folder and the chatbot it updates either in real time or on a schedule that you set and then it's ready to answer your questions using that fresh updated context which is pretty cool, right? JSON file for NA10 is in the description. So, make sure you use that and create your own ragbot. Basically, in a nutshell, rag is making your AI actually know your world. All right, ladies and gentlemen, that's our session for today. Until next time, keep building, keep experimenting, and stay tuned to Builder Central for more such content.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://youtu.be/dQw4w9WgXcQ</t>
+          <t>https://youtu.be/e3MX7HoGXug?si=BK2SOrsETSr0AWLU</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[♪♪♪] ♪ We're no strangers to love ♪ ♪ You know the rules
-and so do I ♪ ♪ A full commitment's
-what I'm thinking of ♪ ♪ You wouldn't get this
-from any other guy ♪ ♪ I just wanna tell you
-how I'm feeling ♪ ♪ Gotta make you understand ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ We've known each other
-for so long ♪ ♪ Your heart's been aching
-but you're too shy to say it ♪ ♪ Inside we both know
-what's been going ♪ ♪ We know the game
-and we're gonna play it ♪ ♪ And if you ask me
-how I'm feeling ♪ ♪ Don't tell me
-you're too blind to see ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ (Ooh, give you up) ♪ ♪ (Ooh, give you up) ♪ ♪ Never gonna give,
-never gonna give ♪ ♪ (Give you up) ♪ ♪ Never gonna give,
-never gonna give ♪ ♪ (Give you up) ♪ ♪ We've known each other
-for so long ♪ ♪ Your heart's been aching
-but you're too shy to say it ♪ ♪ Inside we both know
-what's been going ♪ ♪ We know the game
-and we're gonna play it ♪ ♪ I just wanna tell you
-how I'm feeling ♪ ♪ Gotta make you understand ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪ ♪ Never gonna give you up ♪ ♪ Never gonna let you down ♪ ♪ Never gonna run around
-and desert you ♪ ♪ Never gonna make you cry ♪ ♪ Never gonna say goodbye ♪ ♪ Never gonna tell a lie
-and hurt you ♪</t>
+          <t>All right, builders, let's break down this MCP thing. Model context protocol. You've probably seen the buzz maybe on Twitter, maybe in your dev circles. Everyone's calling it the next big thing. Like literally the future of how LLMs talk to well, you know, everything. Your databases, your apps, your code, even your crazy prompt chains. Think about it. Remember when USBC dropped? Suddenly, one cable to rule them all. charging your laptop, your phone, headphones, connecting displays. Total game changer, right? That's the vibe MCP is going for, but for AI, it wants to be the universal connector. Okay, so we're going to cover three things. First thing is what is MCP and why should you, especially if you're coding, even care. Second is the origin story. How did this become a thing? What's the pain point solving? And the last thing is real world action. We'll jump into Windsor and cursor solid AI dev tools and actually hook something up using an MCP. Sounds good? All right. So, let's dive [Music] in. First is what actually is MCP? So, MCP is equal to model context protocol. A super simple idea but with crazy implications. Think of it as a standardized plug-and-play system for all AI models. GPD4, Claude, Miscrol, whatever, whatever hot new model drops next week. And the reason that these are so important is so that it connects with different data sources, different tools, APIs, you name it. But why now? Let's map the evolution. So, it kind of went through phases, right? So, now let's talk about phase one, just LLMs. This was the start. Chat, GPT, Claude, etc. explode onto the scene. Insanely cool tech. But let's be real, at their core, they're just predicting the next word based on massive training data. On their own, they're kind of dumb. They hallucinate and do some stupid Now, let's move on to phase two. LLM plus context. This is the billion dollar step. Things got way more interesting here. Companies realize LLM plus external stuff is equal to value. For example, Plexity LLM plus web search. Boom. Let's talk about cursor. It's an LLM plus your actual code base, whether it's reading or writing. And this has insane productivity boosts. Let's look at your Gemini tools, which is an LLM plus your Google Workspace, which is your emails, your talks, or your sheets. And suddenly, it's useful for your daily tasks. These aren't just chat bots anymore. They're integrated tools. And that's why they hit those crazy valuations. They solve the context problem. And that means no more manually spoon feeding data from 10 different tabs. And we all know AI is only as good as the context that you give it. Now let's move on to the third phase which is your MCP. Fixing the integration mess. So right now it seems like LLM plus tools equals problem solved. Right? Almost. What's the issue? Scaling this integration is a nightmare. It's a classic N into M problem. You have N AI apps trying to talk to M different tools, databases, APIs and every connection is custom. Connect to Postgress custom code specific authentication. connect to Slack, different API, different framework, different authentication. So even if you want to connect your local file system, you have to take another approach. It becomes a combinatorial explosion for developers and that is absolute chaos to maintain. Sure, we had APIs, web hooks, random frameworks, but it was like having a drawer full of different charger cables for every single device. Fragmented mess. So MCP steps in and says hold up let's just make one standard protocol like USBC which is one way for any AI to get any context that it needs using a defined set of rules. Okay so let's break that down. Let's look at the model any AI model GPT4 claw 3 Gemini future GPT5 text image video models it doesn't matter. Now let's look at the context. The stuff the model needs to be useful. Code from your repo, data from your database, or info from Slack, files from your disk, function calls. Basically, anything that makes the AI smarter for your specific task. A protocol is the standardized rule book, the common language, how the model asks and receives information, how the model asks and receives context. It's not a tool itself. It's the standard everyone agrees to use. Think HTTP for the web. With MCP, your AI can discover and use data sources, local or remote, without you building a million fragile custom integrations, which is huge. Now, we're going to talk about the MCP architecture. Okay, you get the what and the why. Now, how does it actually work under the hood? Super high level, right? Stay with me. MCP client, this is your AI application or agent. Think of it as the brain, the thing that needs data or needs to do something. It's running inside cloud desktop, cursor, windsurf or your custom AI app. It initiates the requests. Now we move on to the MCP server. This is a lightweight helper program and this part knows how to talk to a specific thing using the MCP standard. Got a local database? Run an MCP server that speaks SQL to that database. Want Slack integration? Run an MCP server that talks to the Slack API. If you need access to local files, an MCP server can handle that. Next, we're talking about the data sources and the services. This is the actual stuff that the server connects to. And these are of two types, local and remote. So, let's talk about local first. This includes stuff like your files, databases on your machine, personal APIs that are running locally. And when we're looking at the remote aspect of things, this can be anything on the internet, whether it's Slack, Gmail, Stripe, Notion, GitHub APIs, cloud databases. So, they all communicate using the MCP protocol. The client finds a server that advertises, let's say, GitHub capabilities. The client then tells the server, yo, using MCP rules, create a new repo called awesome project. And then the server goes, I got you, fam. And interacts with the GitHub API and reports back. All right, so it's enough time for theory. Now we're going to jump into it. So let's start by opening up Windsor and then setting up an empty project in a new folder. All right. So once you're in the next step is to go to Windsoroft settings which is down right here and click on the advanced settings option. So in here you'll see cascade and under that you'll see MCP. So go there and see if it has written ad server. Okay. So once you find the ad server click on that and now you'll see a bunch of templates. So for the scope of this video let's add GitHub mainly for two reasons. All right. The first one is we're seeing that GitHub is becoming a nightmare for nontechnical folks. So secondly, it's super super useful for VIP coders who are not technical and still want version control to host using Versel, Netify, etc. So now the setup is relatively simple. Okay, so first what you need to do is create a GitHub account. So for that we're going to go to github.com. Click on the sign up button. Okay, this process is super easy. Takes about a minute. After you sign up, you'll be redirected to the homepage. But as you know, we need to give access to this account to Windsurf. So there must be some sort of linkage going on. So for that linkage, there's something known as personal access tokens. You need to scroll all the way down and find developer settings. Once you click on that and then click on personal access tokens, now you're going to find these fine grade tokens. The reason we chose that is it lets us control how much access MCP has when we add it in windsurf. So all of that is under your control and in order to get control of that you need to do this. So now let's click on fine grained tokens and generate a new token. We're going to name it MCP surf and set the expiration date to this. You can set it to whatever you want. We're going to put it 1 week from now and scroll down. So I'm going to select all the repositories and then we need to select the specific permissions. So this is actually very detailed and you can really spend time thinking okay what do I want to have access to but to keep it simple just follow what we're doing okay administration read and write commit statuses read and write content read and write and issues read and write then after you finish that scroll all the way down and click on generate token again you can set any permissions you want now just click on add server so once you click Click on add server. It's going to ask you for personal access token. Remember this is what we made while making the new account. So take that same access token and put that in over here. This will take a few seconds to connect. That's going to take a couple seconds to connect. And once it's connected, you can create update files, search repositories, create repositories, blah blah blah, all of that stuff. It's pretty impressive, right? So now let's test it out by creating a new GitHub repo. Okay. So, let's simply ask to make a new repo named builders central and see our account is new and doesn't have any repos at all. Okay. Okay. I got one here. So, let's see if this works. Similarly, we have Postgress, we have Stripe, Slack, and many more templates over here. And not just here, you can add hundreds of templates online on sites like Composio, which is like an app store for MCP client etc. how MCP changes the game for VIP coding. I mean, look at this. We just set up a GitHub integration without writing a single line of integration code. We just talked to the AI in plain English. That's the dream of VIP coding, right? Tell the AI what you want and it handles all of the grunt work. The problem was that VIP coding breaks down the moment you need a new tool or data source that AI doesn't know about. You'd obviously hit a wall needing real coding or some hacky workaround. MCP makes VIP coding way more powerful and realistic. You need to orchestrate a workflow across GitHub, Slack, and maybe Stripe. Connect the respective MCP servers. You just need to focus on the what, not the how of the connections. This isn't just for VIP coders, though. Even for experienced developers, this standard potentially simplifies managing tons of integrations, making systems less brittle and easier to scale. But for those of us leveraging AI to build faster, maybe without deep traditional coding skills, MCP is potentially insane. It unlocks the next level of AI orchestration. The more people build and adopt MCP, the faster we get the universal standard. If you're like us and excited about AI doing more than just generating text or code and actually orchestrating tasks across your entire digital life, MCP is something to watch closely. Let me know in the comments. Are you hyped for MCP? All right, so that's the download on MCP from us here at Builder Central. And until next time, keep building.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://youtu.be/5WQgLboa_I8?si=9aa5yYadmRvEzxVn</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Um, let me quickly introduce Natalie Laauo who's going to run our next session. Uh, uh, CEO of the App Inventor Foundation. Yes. Um, that's enough. Yeah. And director. So, come on up, introduce yourself, and, uh, walk us through this next great session. Well, thanks everyone for being here. Thank you. [Applause] So I think echoing the honorable minister from Sarah Leon, today's youth aren't waiting for solutions to be implemented for them. They're creating them themselves and that's what this session is all about. So I'm very very excited to start the global AI hackathon final showcase this year. Uh my name is Natalie. I'm the executive director of the Appmener Foundation. And I think when we talk about the MIT AI and education summit, students are at the heart of all the work that we do and all the research that we do. So I'm really excited to celebrate six amazing student teams from all over the world from six different countries who will be presenting apps that they built with AI to solve community problems in their communities. Uh according to the UNESCO United Nations AI competency framework for students. Uh so I think before we get started I wanted to also acknowledge like the space that we're in today. So this is lecture hall 10250 and it's the second largest lecture hall on MIT's campus. Uh this was also where I took my first AI course as an undergrad at MIT. So that was taught by Professor Patrick Henry Winston who unfortunately is no longer here with us today. But his lessons about how we represent knowledge, how we build robust systems, how we reason through problems, I think are still relevant to AI development today and possibly are even more relevant since the technology is moving so quickly. Um, so to explain the format of today's event, we'll have six teams come up. Each will present their apps and then we have a panel of three judges who will do a short Q&amp;A with them. And then after all of that, they'll go and deliberate in the hall and give out three awards. One for community impact, one for creative innovation, and one for the best design. Uh before I get started with presenting the students, I'd like to introduce Zarin Chowri, who is our program manager for the Apathon and Hackathon programs to tell you a bit more about the larger events that led to today. So please welcome Zaren. [Applause] Okay. All right. Oops. All right. Good morning everyone. Welcome to the global AI hackathon final showcase and awards. Welcome to everyone who's here with us in person at MIT as well as those of us joining virtually via the live stream from all over the world. We're so happy that you're here with us today. When we started the global AI hackathon a year ago, we wanted to create a way for more people to get involved in shaping the future direction of AI. We believe that AI use usage should not be dictated by a small group of researchers or developers working at certain organizations. We think that everyone everywhere should have a say in shaping AI, even and especially the youth. So, we put out a call to anyone around the world to tell us what it would look like to use AI for good in their communities. And boy, did they answer. In fact, we heard from over 1,300 participants this year. That's a 42% increase compared to our inaugural year last year. And not only did the volume of participation increase, but submissions came from all corners of the world. 86 countries and regions to be spec specific of which 60% came from the developing world. The top countries represented were in order the United States, India, Brazil, Singapore, and Indonesia. We are also proud to share that participants ranged from as young as 5 years old all the way to 77 years old with a median age of 17. In this particular session, you'll be hearing from the youth um participants um and right afterwards, we will have the adult participants as well. The theme of this year's competition was the United Nations sustainable development goals or the SGS which in their words are a blueprint for peace and prosperity for people and the planet for years to come. Participants had the choice to address one or more of the 17 SGS in their apps and the most popular ones were good health and well-being, quality education, and climate action. In addition to the SG theme, submissions were also required to use AI in some form. The top three AI categories were generative AI such as chat bots and image bots, classification models such as Teachable Machine, and speech and translation tools like speech to text. You'll notice that the percentages don't quite add up to 100%. That's because most of the submissions use not just one, but actually multiple forms of AI, exploring the interesting intersections and interactions of different AI modalities. Now you might be wondering who are these participants who are building such sophisticated AI apps? Were they already seasoned computer programmers or AI experts? Well, you might be surprised to learn that in fact 90% of our participants were actually beginners to MIT App Inventor. In other words, in their first or second year. This statistic gives us confidence that App Inventor is staying true to its mission of making technology creation accessible for people of all backgrounds so that someone can go from being a mere beginner to programming to developing their very own AI AI app in just a year. And we actually quantified that impact after completing the competition. 95% of participants now feel that they have the potential to positively impact their communities by creating AI apps. That's powerful. We were floored by the quality and impact of the submissions and we thank every participant for bringing their creativity and innovation to this competition. We also want to thank our 53 judges who spanned from MIT App Inventor power users to teachers and industry experts. I also want to shout out that we launched a new pilot mentorship program this year in partnership with Braise um in which we paired our finalists with mentors in order to prepare for their presentations. We want to thank our volunteer me mentors, half of whom came from the mi from the app inventor team and half of whom came from our partner brace. We are so inspired by the success of this year's competition and we are eager to see what the future holds. We have already expanded our global AI hackathon program by launching regional programs in Taiwan and Japan and we look forward to growing our Apathon offerings in the years to come. Thank you so much for listening and let's hear some great student presentations. [Applause] Thank you so much, Zaren. She also put so much work into this aathon over the past two years. So when you see her afterwards, tell her thank you for me as well. Um, so now I'd like to introduce our three judges. First we have Rod McCloud, who is the vice president of social impact at Braise. Please come up and take a seat. Thank you. We also have Kelly Shiohira who is the lead expert on the UNESCO AI competency framework for students. And finally we have Mark Freriedman who is co-founder of the app amentor project at Google and is now MIT CCL research affiliate. He uh co-founded App aimemen with professor Hal Abson of MIT 15 years ago and this project has reached 24 million learners around the world. So thank you Mark. So now I'd like to invite our first project up uh rehab AI. [Applause] Hello everyone. My name is Cody Lee and I'm extremely honored to present my project rehab AI, an app designed to make TA rehab more efficient for patients and doctors. In this presentation, I'll cover the problem, the app design, app features, and finally the potential impact in the summary. Let's start off with the problem. The American Hospital Association predicts that there will be a healthcare shortage of 124,000 physicians by 2033 and it's already affecting healthcare today. One sector heavily impacted is TA rehab. Teler rehab or online rehab allows patients to meet with doctors virtually and complete rehab exercises from home. For patients who live far away from hospitals or have difficulty moving, TA rehab can be lifechanging. As you can see, demand for TA rehab has grown rapidly with the market expected to reach 17 billion within the next 10 years. But as demand grows, burnout causes wickers to quit, which strains the system and causes more and causes delays in vital patient care. To close the gap, I've created Rehab AI, an app designed to solve this problem by using AI to make Tel Rehab more efficient. Using the camera of the device, rehab AI can track, classify, and score rehab exercises patients perform so doctors can monitor them outside of meetings. To see this, let's go into the app design. Rehab AI is split into a patient user interface and a doctor's user interface with data transferred through cloud servers. Rehab AI has three core components. the post model, evaluation model, and communications module. First, the post model, which is located on the mobile device, detects key points on a person's body. Then, the app transfers the data to the evaluation model. The evaluation model calculates joint angles from the postnet key points. Angle measurements in rehab exercises have different patterns over time which can be analyzed by using AI. The AI I've selected is a LSTM neuronet network. It is highly effective at classifying time sequence data making ideal for analyzing movement patterns. In this rehab exercise, I designed and trained my LSTM neural network on mat lab and achieved a classification accuracy of 98% across all nine exercises. Here shows the classification and evaluation in real time. In the meantime, the results are sent back to the doctor uh sorry to the app for display. Let's take a look at this in the app's features. When logging in as a doctor, they'll see a list of patients. Clicking on one, they can see their workout history. They can set reminders and assign new tasks. Logging in as a patient, they can see the patient homepage. Patients can click on assignments to see doctor's feedback. and clicking on info, they can see detailed exercise descriptions and video clips of each exercise. To wake out, patients press wake out and start positioning themselves in front of the camera. The AI will track the squat. The AI will track the exercise and classify it by announcement. In the app, they can see the detected exercise and the score. Patients can also add a video overlay over the key points. Once they're done, they press stop and they can see a detailed summary of their workout, including the scores and duration of each exercise. And now, let's wrap up with the summary. Rehab AI aims to reduce the burden on healthcare workers while improving care for patients. It shows how we can use AI to solve realworld problems as plenty of room to improve in the future. This project isn't just about AI. It's about using AI to make a meaningful impact on people's lives. And with that, thank you so much. [Applause] Uh I'm just wondering what got you interested in this problem. It's not something that would come naturally I would think. So what what got you interested? Mhm. So I did some projects in the past relating to the pose model and it was really interesting on how it classified movements. So um classified like results and like sees how movements can displayed on AI and I really got into rehab after my my some of my relatives were also in this physical rehab industry and that just really I just wanted to mind how to use the post model to really uh classify and evaluate these results. Um, and curious if you've done any testing with this app, if you've had use cases, family members, friends, for example, any feedback, both positive and negative, you got from that testing. Uh-huh. So, uh, some family and friends all tested the app. They said it pretty worked pretty well, but there were some improvements that could be made to make it even better. One major key thing that I've heard was to diversify the data set. So I've trained this um I had training data of 30 minutes of each exercise and each exercise I tested on various family members big and small to try to diversify the data set as best as possible. However, we can expand on this by taking people, many people to get the AI to generalize them better and to classify it even more. Just a quick followup. Did you test on actual rehab patients or were these like fully healthy adults who were testing it? They're fully healthy. Yeah. So um so in this case I'm just wondering if um you know when you're in rehab you don't perform the motions exactly exactly so does your model um account for this sort of discrepancy in what for example someone with a shoulder injury can't do like a full lift or something and how how does that work exactly? Mhm. So in our app there's not only once you're finished with the exercise you not only see the duration of each exercise but also the score. What that means is how accurately is it being done. Yeah. Yeah. So patients who cannot perform the whole motion they will the exercise will be detected. However the score wouldn't be the highest. So the doctor can look at the results through doctor supervision and actually see where the patient is struggling on and where the patient is best at. Thank you. Someone who's been in rehab. [Applause] All right. Thank you so much Cody. Uh, now we have the move to heal team from Turkey. Oh no, it buddy. Sorry, it's kidney buddy. Sorry. You're after. I think I have an old Yeah. Thanks. There's extra mics here if you guys Okay. Yeah, I have no idea. Oh, it is that one. Ready? [Music] Oh, man. This one is on. How do you know if it's on? Okay. Oh, it's on. Okay. Good morning, everybody. All right. So, me, my name is Alan Zang. I'm here with my teammates today, Alina, Isabelle, and Alec. And we are here today to introduce our app, KY, which is the first AI powered app for chronic kidney disease, or also known as CKD Care. Just to give some background info in the US about 35.5 million adults have CKD and this risk substantially increases with age as between the age groups of 18 to 64 we have about 18% while those over 65 plus have about 34% which is about 1 in three seniors and so due to the fact that there's so many seniors who have CKD we this really highlights the urgent need for better management tools for those people. Unfortunately, our grandma is one of the people affected by CKD. Every meal is an uphill battle for her because she needs to meticulous meticulously track her daily nutrient intake which causes a lot of stress for everyone involved. So, as we were observing her CKD journey, we noticed three big problems. The first is the disjointed and generic tools. Um the available tools on the market right now are fragmented and not comprehensive causing many patients and users of the apps to um jump between the different apps. Secondly, these other apps can also cause exhausted users and caregivers. Seniors struggle with complicated apps and caregivers are often overwhelmed trying to help them juggle meals, medications, and appointments every day. Third, there are also support gaps and rising costs. Uh one critical thing is that oftent times uh doctors aren't able to have access to patients progress info such as daily nutrient tracking and what results is that they can miss early warning signs which leads to delayed care and therefore uh rising healthcare costs for those individuals and so this is why we created Kenny Buddy for our grandmother and other family like ours. Kidney buddy has many technological components such as MIT app inventor of course and smart AI like chatbt plus the additional speech recognition and text to speech. It makes it super easy to use and truly senior friendly. CKD gets worse over time and can cause kidney failure or early death. There's no cure, so managing protein, potassium, and phosphorus is key to protecting the kidneys. And this is why our app help track these three Ps to help better management and help a healthy kidney. And additionally, you're able to get friendly CKD meal planners for all CKD stages. And you are able to track through video, text or photo which makes it easier to track key nutritions. And if you see the limit, it will send an alert. Kenny Buddy also helps um in other ways such as you're able to assess your CKD risk easily to support proactive prevention, find any nearby doctors and labs, answer any questions you may have on CKD, and the app will also send you AI powered reminders. Additionally, it p it provides detailed AI powered progress reports for 7, 30, 60, and 365 days. It's able to, you know, track the trends over time and generate reports for doctors to solve the issue of the disjointed and fragmented tools. Um, Kinyuddy is an all-in-one AI powered uh device that is both intuitive in its uses and comprehensive in its applications. To prevent exhausted users and caregivers, our app uses chat GBT with a texttospech interface making it senior friendly. These features can also help caregivers stay organized with progress tracking and appointments. uh in order to solve the issue of support gaps and rising costs, we decided to use AI uh in order to help doctors be able to track those uh progress reports which allows them to detect those uh early uh signs of the disease and then in addition to that help them uh decrease the amount of time between initial care and therefore decrease healthcare costs for the individuals. Now onto the global impact. According to our research, 850 million people worldwide are affected by CKD. So it hits underserved communities the most and medically disadvantaged communities as well. But with Kennybody, we can increase better outcomes and have better um healthcare all around the world. Uh this is some comments and feedback from my grandmother and so my grand my my grandparents said that uh we made this app to help her with her CKD and overall it has made her feel much better, happier and more in control. We also have comments from anologist in general. He said that because um proper diet management is key to um like maintaining your kidney health since our app helps with um meal planning and tracking your nutrients. It is a great app that he suggests his patients to use daily. Kidney brings empathy AI and clarity all around the world. I hope you like their app a lot. Thank you. So, so I'll ask uh it's great that you tested it with your grandmother. Uh but did you manage to test it with uh any uh seniors who you were not related to? Uh yes, we tested with our neighbors actually cuz they're seen like they're older. I think they're I won't guess their age, but I think they're above 50. Um and we definitely we definitely tested with um other family members too as well. Um and they gave us good feedback. They also gave us tips um what needed to be changed and we fixed a lot of bugs and stuff throughout the whole process. And did they find it to be stressfree? Uh definitely because you know as I mentioned you know you can uh track it by voice text and photos which makes it super easy and super senior friendly. Um, and curious if you've defined key metrics for for this app in particular. Um, obviously your grandmother want to live a healthier life, a longer life. That's kind of hard to track and measure. So, how do you think about metrics? Um, wait, wait, sorry. In in terms of your app, how do you know if it's successful? If the users are having a good experience, is it based on user engagement scores? Uh, definitely seeing improvement over time. um seeing if they you know they're feeling better, their the healthy are better. We go to the doctors for checkups, see if they're, you know, maintaining their meds, eating the right foods. Um and definitely seeing over the app um the progress of detail reports, seeing that they um increased a lot of um their and like they they make sure they're they didn't go over their uh key nutrition intakes from the three Ps. Thank you. All right. Now, please welcome Move to Heal. [Applause] You want to use Hello everyone. Today we're excited to present Move to Heal, which is an AI powered mobile app created to make home rehabilitation simpler, safer, and more accessible for people recovering on their own. We're a team of five high school students from Turkey, freshman, and sophomores, and we are proud to be this year's MIT EP Inventor Global AI hackathon team winners. We're all part of robotics team and patient about AI and technology. I'm DNA. In this project, I worked on posnet development and created our demo videos. Baton integrated our posnet and created our K features. Ada used on Ada created our chatbot. Dennis helped us to build UI and Ail created the user experience. Okay. Aligned with the United Nations sustainable development goal three, good health and well-being, our mission begins with a pressing reality. Around 2.4 billion people, nearly the one-third of the world, need rehabilitation. This number has grown by 63% over the past 30 years, and it continues to rise. Yet, only one in 10 has access to proper care. And for those trying to recover at home, 65% perform their exercises incorrectly, risking further injury. True healing is far more difficult to achieve under these conditions. And behind all these numbers, there are real people. For us, one of them was my grandmother. Seeing her try to keep up with rehab in pain, confused, and completely alone was really hard. She and so many others going through the same thing desert the weather. And that's what pushed us to develop something that could actually help. Now, let's take a look at what Motill offers. Our app uses AI to support users during their rehabilitation at home. It's built around a simple user-friendly interface and provides a safe experience by prioritizing security and privacy. Users can track their progress over time, receive real-time feedback for uh their exercises, and even save their favorite routines for easy access. Altogether, these features make move not just a tool, but also a supportive companion throughout the recovery journey. You can watch a tutorial video before getting started and then perform the exercise while receiving real-time feedback from our AI model. You can track your progress by viewing your exercise history by by adding the exercise you want to your favorites list. You can access to it anytime you want. Additionally, your personal AI assistant Moa is here to support you through your recovery journey. Here's a simple diagram showing how the core parts of our app are structured. After logging in, users land on the homepage where they can access three main features. Favorites, chatbot, and history. In favorites, selected exercises are saved using tiny DB1 and showed based on button visibility. Our chatbot handles user input, inject system message, and shows responses creating a smooth interaction flow. And finally, the history screen starts previously completed exercise again using Tiny DB1. This structure allowed us to keep the user experience simple while making sure K features are accessible at all times. One of the key features of our app was the combination of a personal image classifier and a poset extension. Briefly, personal image classifier is an image processing unit provided by MIT app inventor and posnet is an extension that we use to extract the patient's skeleton from the image to reduce environmental factors. By using these link units, we were able to achieve great accuracy in the test sets that the experts we interviewed provided. And in our journey to make home rehabilitation safer and more accessible, one of the most significant milestone was meeting MIT epimementor. MID MIT Appmentor provided us an easy and global way to create and expand our app. even global enough to share it in the MIT. Our app is built around three core principles, privacy, safety, and fairness. It includes a simple login page for data protection and brief medical disclaimers for safety. But most importantly, we reduce bias using poset to extract the skeleton instead of analyzing the raw images. So our AI model, personal image classifier model only focuses on the movement, ignoring irrelevant factors like skin tone, body shape, lighting, and background. Our biggest strength, real time feedback that helps users correct mistakes right when they happen. Our interface is simple, friendly, and uh designed for everyone, not just tech experts. Yes, we're still growing. We're working with a small data set, and we haven't reached clinical validation yet, but the opportunity ahead is massive. uh millions need support and we are uh building a solution yet that can truly reach them. As a team we have built a strong foundation but we know there's a still long way to go. Our next steps start with expanding our data set to improve model performance. Then we aim to begin a medical collaboration so we can collect real world feedback and improve realability. After that we will move into clinical validation working with professionals to test the app in real scenarios. And finally, once we are confident in its accuracy and safety, we will prepare for an official avalanche. We believe each of these steps will bring us closer to make a real world impact. We'd like to thank Dr. Fatma Pinayish, Dr. Murat Shahin, Dr. Sichil Kind, and our project advisor Oankus for their immersive support which truly enriched our project. These are resources we use throughout our project. We're not redesigning rehabilitation. We are redesigning what it means to be supportive when you need it most. And thank you for listening to us. You can contact us for more information. [Applause] So, apologies if I missed it. Um, and I do understand that one of your next goals is to expand your data set. Could you just elaborate a little bit on your initial data and where that came from? Um we trained our AI models with images taken from the posnet uh and we have nine different AI models uh for nine different exercises. Um in the AI models uh we trained uh we have 200 images per AI models and 100 images per uh classes. So in total we have um 1,800 images in our data set. Uh and I'm I'm curious uh you clearly work with medical professionals on this. So curious what their feedback is and any user feedback you've received throughout this process. Um you can. Yeah. So um her grandma uh tried our app and she also told that it's very simple to do. So um it was very uh good for her to try that. Um and if we talk about the experts um we had two um rehab experts. Sorry for our English by the way. We have two AI experts. sorry, rehab experts who helped us through the uh sharing um the data set sheets for rehabs and um giving feedbacks for us and organizing meetings with um other patients that we can try our project. And additionally um we had a AI expert who helped us uh about uh giving feedbacks um which consists u adding um demo videos to our app and um some opinions about the UI. Okay. Thank you so much. Thank you. Additionally, we want to thank our mentor who helped us through the um preparing the presentation, Salem TZ. Thank you so much. All right. Thank you. Um and also please don't apologize for your English. It was a fantastic presentation and I could not speak this well in a second language. Uh so next I'd like to invite Cho Cook. [Applause] Thank you. Hello everyone. I am Hannah. I come from a tiny city 60 miles north of Tokyo. It's famous for strawberries. First of all, thank you very much for giving me this wonderful opportunity. The reason I decided to create an app was because I opened the fridge one day and I found this watery roten tofu. I was like, "No, I wanted to use that for lunch." I showed it to my mom and no, I showed it to my mom and she was like, "Oh, no. Not again. How many times how we let stuff go past its expiry date? My mom is great at making well balanced meals, but she always ask me and my little brother and sister. What should I make for dinner? And we are like, "It's up to you." Nobody has any ideas. And if my mom's dinner is the same as the school lunch, my little brother and sister like this again, we had this at school for lunch. That made me think, we need a nap. I thought, wouldn't it be great if there was a nap that turned a list of ingredients into recipes? So, I made one. It's called Chuk. The name comes from combining the Japanese word chto meaning just a little and the English word cook expressing the hope for a future cooking can be done easily and quickly and you can even add more ingredients by taking more photos of different receipt. Last month I did a try of the app at my local library. People suggested using the supermarket fryers or handwritten list of leftovers. You, for example, you could you could take a photo of sale items and get recipes using just those discounted items or recipes just need one or two other ingredients. The AI engine can easily come up with dishes you don't usually make, so your kids won't say things like, "Ah, we had this at school for lunch." Then you can spend more time doing the things you love like going out with your family and participating in seasonal events like the cherry blossom festival in my town. These events helped to revitalize towns. Now we face global challenges as outlined in the SDGs the sustainable development goals. One of these goals includes reducing food waste. In Japan, about 6 million tons of food went to waste in 2019. Of that, about 2.76 million tons came from households. Globally, about 1.3 billion tons of food was discarded in 2019 with 931 million tons being classified as food waste. Despite all the food wasted about 650 million people was were suffering from hunger in 2019. Social conditions certainly add to hunger and we must remember that no one chooses the country or environment they born into. Knowing that there are people in difficult situations. I want to do everything I can to help people in need around the world. In conclusion, Chook is not just a recipe app. It creates conversations, saves time, and helps build small connections in our daily lives. The reason I'm able to stand on this today is because of the incredible support I've received from the people in my local community. I hope that Chuk, which was inspired by my mother's struggles, will be helpful to her and who has support and to everyone who has supported me and to Japan's efforts in reducing food waste. and eventually I hope it brings smiles to people around the world. Thank you for your attention. [Applause] So I will um I will ask my question in Japanese if that's okay. I asked her uh if she got any feedback from the people at the library about things to improve or change about her app. Um, one people said me, I want to add more ingredient more receipts in um, I want to add more ingredients and more I want to talk I want to take more pictures not only one pictures two or three. So please change the the program and so the one people want want to see how to use this app. So I make a page of manual. I understand. Um and curious who who is your target user? Is it um a main cook of a household or like you know target user? My my mother's or my who makes dinner or what who doing the cooking. Okay. No problem. Uh, next we'll have Eeky Guy for teens. And uh I think the clicker is broken, by the way, so you'll have to tap on the arrows. I'll I'll show you when you get down here. Thank you. Can we connect our Yes. There's a little We have a We have one. You have your Yes. Hi, I'm Victor. Hi, I'm Ronald. Hi, I'm the Musa. I'm sure many of you have always started that stage of life that you don't quite know what you want to do and you're trying to find yourself, but everyone's telling you what you should be, parents, teachers, and we're currently in that stage. So, we decided to invent an app to fix our problem. We developed Iky Guy for teens, a self-discovery and career planning app. Did you know that over three4s of high school seniors are unsure what career they will enter after college? And over half of juniors say that they regret not planning earlier as freshman and sophomores. This is because there's a lack of support for career planning for teens. One reason for this is that teens are often unwilling to communicate their career plans with their parents. In the case of first generation students, their parents may be unable to assist in planning. And in other cases, the students fear that they'll be forced into a career path by their parents that they do not enjoy. Furthermore, most current career planning tools are not holistic and only focus on a single factor. When I asked my classmates and friends about what they thought about curre</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://youtu.be/CF52N-w4anI?si=6f8tnZm1ydqOpOkt</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>अगर आप लोग एआई एरा में प्रोग्रामिंग करना चाहते हैं, तो कौन सी प्रोग्रामिंग लैंग्वेज आप लोगों को अपनी फर्स्ट प्रोग्रामिंग लैंग्वेज के तौर पर चूज़ करनी चाहिए, यह मैं आप लोगों को इस वीडियो में क्लियर करूंगा। मैं इस वीडियो में स्टूडेंट साइकोलॉजी को ब्रेकडाउन करूंगा और आप लोगों को एक ऐसी चीज बताऊंगा जो कि शायद आपको 3 साल बाद, 5 साल बाद या 7 साल के बाद रियलाइज हो। कुछ चीजें आप लोग अपने करियर पॉइंट में जितनी जल्दी समझ जाए उतना बढ़िया है। तो चलो स्टार्ट करते हैं। सबसे पहले आप लोग कौन सी प्रोग्रामिंग लैंग्वेज चूज़ करने वाले हो। यह डिपेंड करता है कि आप अपनी लाइफ में क्या करने वाले हो। अगर आप लोग डेटा साइंटिस्ट हैं तो मे बी आप लोग पाइथon से स्टार्ट करना चाहें। अगर आप लोग एक वेब डेवलपर हैं तो आप जावास्क्रिप्ट से स्टार्ट करना चाहें। आप अगर ऐप डेवलपमेंट करना चाहते हैं लेट अस से आप स्पेसिफिकली आप लोग फ्लटर एंड आर्ट से वेब डेवलपमेंट करना चाहते हैं तो आपको डार्ट सीखनी चाहिए। बट अगेन लोग बहुत ज्यादा कंफ्यूज हो जाते हैं इन चीजों को लेके और मैं आप लोगों को बताता हूं कि क्यों आप लोगों को यह डिसाइड करना प्रायोरिटाइज नहीं करना चाहिए कि मेरी प्रोग्रामिंग लैंग्वेज कौन सी होने वाली है। रादर आपको यह प्रायोरिटाइज करना चाहिए कि आप अपने करियर में करना क्या चाहते हैं? मैंने देखा है बहुत सारे स्टूडेंट्स से जब यह पूछा जाता है कि आप क्या हैं? हु आर यू? क्या आप एक डेटा साइंटिस्ट हैं? क्या आप एक वेब डेवलपर हैं? कि उनके पास आंसर ही नहीं होता है। ज्यादातर लोग कहते हैं कि यार मैं तो सब कुछ कर लेता हूं या थोड़ा-थोड़ा सब कुछ कर लेता हूं। एंड ये एक बहुत बड़ी प्रॉब्लम है। एi एरा में अगर आप लोग सक्सीड करना चाहते हैं तो जो बार है ना वो रेज हो चुका है। अब ऐसा नहीं है कि आपको थोड़ी बहुत पाइथन आती है तो आप एक कोने में ल</t>
         </is>
       </c>
     </row>

</xml_diff>